<commit_message>
feat(employee): import employee with relation
</commit_message>
<xml_diff>
--- a/public/assets/templates/employee_multiple.xlsx
+++ b/public/assets/templates/employee_multiple.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>NIK</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>PTKP</t>
+  </si>
+  <si>
+    <t>ID Posisi Jabatan</t>
+  </si>
+  <si>
+    <t>ID Level Jabatan</t>
+  </si>
+  <si>
+    <t>ID Status Karyawan</t>
+  </si>
+  <si>
+    <t>ID Kantor/Cabang</t>
+  </si>
+  <si>
+    <t>ID Divisi</t>
   </si>
 </sst>
 </file>
@@ -387,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,9 +424,14 @@
     <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -456,6 +476,21 @@
       </c>
       <c r="O1" t="s">
         <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>